<commit_message>
Updated csv and xlsx for QEST23 results
</commit_message>
<xml_diff>
--- a/results/qest23/results.xlsx
+++ b/results/qest23/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="39">
   <si>
     <t xml:space="preserve">STAMINA 2.0 (PRISM)</t>
   </si>
@@ -30,9 +30,6 @@
     <t xml:space="preserve">STAMINA 2.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Overlap</t>
-  </si>
-  <si>
     <t xml:space="preserve">Model</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t xml:space="preserve">Window</t>
   </si>
   <si>
-    <t xml:space="preserve">Pmax (S)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Circuit 010 to 100</t>
   </si>
   <si>
@@ -109,6 +103,12 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larger Iteration Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iterations needed (for w &lt;= 10^-3)</t>
   </si>
   <si>
     <t xml:space="preserve">STAMINA 2.0 (Storm)</t>
@@ -150,7 +150,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -197,6 +197,20 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -212,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -268,24 +282,6 @@
       <top style="medium">
         <color rgb="FF9DC3E6"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -360,16 +356,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -378,6 +370,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -465,20 +461,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,39 +486,33 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.395048521778638</v>
@@ -533,40 +524,20 @@
         <f aca="false">C3-B3</f>
         <v>6.66873995179285E-005</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="0" t="n">
         <v>0.395050929649</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="0" t="n">
         <v>0.395100628307</v>
       </c>
       <c r="G3" s="6" t="n">
         <f aca="false">F3-E3</f>
         <v>4.96986579999748E-005</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <f aca="false">F3&gt;=B3</f>
-        <v>1</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <f aca="false">E3&lt;=C3</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <f aca="false">AND(E3&gt;B3,F3&lt;C3)</f>
-        <v>1</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <f aca="false">AND(B3&gt;E3,C3&lt;F3)</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <f aca="false">OR(J3,K3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0165944663225085</v>
@@ -578,40 +549,20 @@
         <f aca="false">C4-B4</f>
         <v>0.00018896416386828</v>
       </c>
-      <c r="E4" s="7" t="n">
-        <v>0.016505543507</v>
-      </c>
-      <c r="F4" s="8" t="n">
-        <v>0.018699379621</v>
+      <c r="E4" s="0" t="n">
+        <v>0.016474768099</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.020078199188</v>
       </c>
       <c r="G4" s="6" t="n">
         <f aca="false">F4-E4</f>
-        <v>0.002193836114</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <f aca="false">F4&gt;=B4</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <f aca="false">E4&lt;=C4</f>
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <f aca="false">AND(E4&gt;B4,F4&lt;C4)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <f aca="false">AND(B4&gt;E4,C4&lt;F4)</f>
-        <v>1</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <f aca="false">OR(J4,K4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.003603431089</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.0166272431867862</v>
@@ -623,40 +574,20 @@
         <f aca="false">C5-B5</f>
         <v>0.000195723126734156</v>
       </c>
-      <c r="E5" s="7" t="n">
-        <v>0.016536754574</v>
-      </c>
-      <c r="F5" s="8" t="n">
-        <v>0.018790310621</v>
+      <c r="E5" s="0" t="n">
+        <v>0.016504701614</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.020246672663</v>
       </c>
       <c r="G5" s="6" t="n">
         <f aca="false">F5-E5</f>
-        <v>0.002253556047</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">F5&gt;=B5</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <f aca="false">E5&lt;=C5</f>
-        <v>1</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <f aca="false">AND(E5&gt;B5,F5&lt;C5)</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <f aca="false">AND(B5&gt;E5,C5&lt;F5)</f>
-        <v>1</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <f aca="false">OR(J5,K5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.003741971049</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.694656523286798</v>
@@ -668,40 +599,20 @@
         <f aca="false">C6-B6</f>
         <v>0.000152241206120674</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="0" t="n">
         <v>0.694661414548</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="0" t="n">
         <v>0.694745396062</v>
       </c>
       <c r="G6" s="6" t="n">
         <f aca="false">F6-E6</f>
         <v>8.398151400002E-005</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">F6&gt;=B6</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <f aca="false">E6&lt;=C6</f>
-        <v>1</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <f aca="false">AND(E6&gt;B6,F6&lt;C6)</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <f aca="false">AND(B6&gt;E6,C6&lt;F6)</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <f aca="false">OR(J6,K6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.455029707750434</v>
@@ -713,40 +624,20 @@
         <f aca="false">C7-B7</f>
         <v>9.06176145982762E-005</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="0" t="n">
         <v>0.455034655826</v>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="0" t="n">
         <v>0.455085701619</v>
       </c>
       <c r="G7" s="6" t="n">
         <f aca="false">F7-E7</f>
         <v>5.10457930000263E-005</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">F7&gt;=B7</f>
-        <v>1</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <f aca="false">E7&lt;=C7</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">AND(E7&gt;B7,F7&lt;C7)</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <f aca="false">AND(B7&gt;E7,C7&lt;F7)</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <f aca="false">OR(J7,K7)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.735722566875715</v>
@@ -758,40 +649,20 @@
         <f aca="false">C8-B8</f>
         <v>0.000123469576992052</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="0" t="n">
         <v>0.735725863933</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="0" t="n">
         <v>0.735790289053</v>
       </c>
       <c r="G8" s="6" t="n">
         <f aca="false">F8-E8</f>
         <v>6.44251200000445E-005</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <f aca="false">F8&gt;=B8</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <f aca="false">E8&lt;=C8</f>
-        <v>1</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <f aca="false">AND(E8&gt;B8,F8&lt;C8)</f>
-        <v>1</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <f aca="false">AND(B8&gt;E8,C8&lt;F8)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <f aca="false">OR(J8,K8)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.826019152979041</v>
@@ -803,40 +674,20 @@
         <f aca="false">C9-B9</f>
         <v>0.000140142121880404</v>
       </c>
-      <c r="E9" s="7" t="n">
-        <v>0.825704905869</v>
-      </c>
-      <c r="F9" s="8" t="n">
-        <v>0.826679465675</v>
+      <c r="E9" s="0" t="n">
+        <v>0.825468466575</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.827041855286</v>
       </c>
       <c r="G9" s="6" t="n">
         <f aca="false">F9-E9</f>
-        <v>0.000974559805999919</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <f aca="false">F9&gt;=B9</f>
-        <v>1</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <f aca="false">E9&lt;=C9</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <f aca="false">AND(E9&gt;B9,F9&lt;C9)</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <f aca="false">AND(B9&gt;E9,C9&lt;F9)</f>
-        <v>1</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <f aca="false">OR(J9,K9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0015733887110001</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.989516178692955</v>
@@ -848,40 +699,20 @@
         <f aca="false">C10-B10</f>
         <v>0.000226782770492484</v>
       </c>
-      <c r="E10" s="7" t="n">
-        <v>0.989293759947</v>
-      </c>
-      <c r="F10" s="8" t="n">
-        <v>0.990188233161</v>
+      <c r="E10" s="0" t="n">
+        <v>0.989230850004</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.990289532157</v>
       </c>
       <c r="G10" s="6" t="n">
         <f aca="false">F10-E10</f>
-        <v>0.000894473214000047</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <f aca="false">F10&gt;=B10</f>
-        <v>1</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <f aca="false">E10&lt;=C10</f>
-        <v>1</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <f aca="false">AND(E10&gt;B10,F10&lt;C10)</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <f aca="false">AND(B10&gt;E10,C10&lt;F10)</f>
-        <v>1</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <f aca="false">OR(J10,K10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.00105868215299998</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99023568796506</v>
@@ -893,40 +724,20 @@
         <f aca="false">C11-B11</f>
         <v>0.000237217126256906</v>
       </c>
-      <c r="E11" s="7" t="n">
-        <v>0.990015119309</v>
-      </c>
-      <c r="F11" s="8" t="n">
-        <v>0.990911760692</v>
+      <c r="E11" s="0" t="n">
+        <v>0.990019346074</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.990893278886</v>
       </c>
       <c r="G11" s="6" t="n">
         <f aca="false">F11-E11</f>
-        <v>0.000896641383000052</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <f aca="false">F11&gt;=B11</f>
-        <v>1</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <f aca="false">E11&lt;=C11</f>
-        <v>1</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <f aca="false">AND(E11&gt;B11,F11&lt;C11)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <f aca="false">AND(B11&gt;E11,C11&lt;F11)</f>
-        <v>1</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <f aca="false">OR(J11,K11)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.000873932811999989</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.864410882646364</v>
@@ -938,40 +749,20 @@
         <f aca="false">C12-B12</f>
         <v>5.36123923586818E-005</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="0" t="n">
         <v>0.86441763714</v>
       </c>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="0" t="n">
         <v>0.864456067813</v>
       </c>
       <c r="G12" s="6" t="n">
         <f aca="false">F12-E12</f>
         <v>3.84306730000228E-005</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <f aca="false">F12&gt;=B12</f>
-        <v>1</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <f aca="false">E12&lt;=C12</f>
-        <v>1</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <f aca="false">AND(E12&gt;B12,F12&lt;C12)</f>
-        <v>1</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <f aca="false">AND(B12&gt;E12,C12&lt;F12)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <f aca="false">OR(J12,K12)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.85743647460294</v>
@@ -983,40 +774,20 @@
         <f aca="false">C13-B13</f>
         <v>6.83981047701065E-005</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="0" t="n">
         <v>0.857436474618</v>
       </c>
-      <c r="F13" s="8" t="n">
+      <c r="F13" s="0" t="n">
         <v>0.857504872723</v>
       </c>
       <c r="G13" s="6" t="n">
         <f aca="false">F13-E13</f>
         <v>6.83981050000337E-005</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <f aca="false">F13&gt;=B13</f>
-        <v>1</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <f aca="false">E13&lt;=C13</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <f aca="false">AND(E13&gt;B13,F13&lt;C13)</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <f aca="false">AND(B13&gt;E13,C13&lt;F13)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <f aca="false">OR(J13,K13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.989490726101482</v>
@@ -1028,40 +799,20 @@
         <f aca="false">C14-B14</f>
         <v>0.00031191727877089</v>
       </c>
-      <c r="E14" s="7" t="n">
-        <v>0.989271919304</v>
-      </c>
-      <c r="F14" s="8" t="n">
-        <v>0.990226828364</v>
+      <c r="E14" s="0" t="n">
+        <v>0.98902501067</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.990641892807</v>
       </c>
       <c r="G14" s="6" t="n">
         <f aca="false">F14-E14</f>
-        <v>0.000954909059999953</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">F14&gt;=B14</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <f aca="false">E14&lt;=C14</f>
-        <v>1</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <f aca="false">AND(E14&gt;B14,F14&lt;C14)</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <f aca="false">AND(B14&gt;E14,C14&lt;F14)</f>
-        <v>1</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <f aca="false">OR(J14,K14)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.00161688213699995</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.498962403458025</v>
@@ -1083,30 +834,10 @@
         <f aca="false">F15-E15</f>
         <v>6.11917199999645E-006</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <f aca="false">F15&gt;=B15</f>
-        <v>1</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <f aca="false">E15&lt;=C15</f>
-        <v>1</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <f aca="false">AND(E15&gt;B15,F15&lt;C15)</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <f aca="false">AND(B15&gt;E15,C15&lt;F15)</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <f aca="false">OR(J15,K15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.499263342110593</v>
@@ -1128,30 +859,10 @@
         <f aca="false">F16-E16</f>
         <v>6.31890199997986E-006</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <f aca="false">F16&gt;=B16</f>
-        <v>1</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <f aca="false">E16&lt;=C16</f>
-        <v>1</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <f aca="false">AND(E16&gt;B16,F16&lt;C16)</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <f aca="false">AND(B16&gt;E16,C16&lt;F16)</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <f aca="false">OR(J16,K16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -1173,30 +884,10 @@
         <f aca="false">F17-E17</f>
         <v>0</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <f aca="false">F17&gt;=B17</f>
-        <v>1</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <f aca="false">E17&lt;=C17</f>
-        <v>1</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <f aca="false">AND(E17&gt;B17,F17&lt;C17)</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <f aca="false">AND(B17&gt;E17,C17&lt;F17)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <f aca="false">OR(J17,K17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -1218,30 +909,10 @@
         <f aca="false">F18-E18</f>
         <v>0</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <f aca="false">F18&gt;=B18</f>
-        <v>1</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <f aca="false">E18&lt;=C18</f>
-        <v>1</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <f aca="false">AND(E18&gt;B18,F18&lt;C18)</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <f aca="false">AND(B18&gt;E18,C18&lt;F18)</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <f aca="false">OR(J18,K18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1263,35 +934,15 @@
         <f aca="false">F19-E19</f>
         <v>0</v>
       </c>
-      <c r="H19" s="0" t="n">
-        <f aca="false">F19&gt;=B19</f>
-        <v>1</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <f aca="false">E19&lt;=C19</f>
-        <v>1</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <f aca="false">AND(E19&gt;B19,F19&lt;C19)</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <f aca="false">AND(B19&gt;E19,C19&lt;F19)</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="0" t="n">
-        <f aca="false">OR(J19,K19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="9" t="n">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7" t="n">
         <v>0.865393695562323</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="7" t="n">
         <v>0.865546456027709</v>
       </c>
       <c r="D20" s="0" t="n">
@@ -1308,35 +959,15 @@
         <f aca="false">F20-E20</f>
         <v>1.57040610000436E-005</v>
       </c>
-      <c r="H20" s="0" t="n">
-        <f aca="false">F20&gt;=B20</f>
-        <v>1</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <f aca="false">E20&lt;=C20</f>
-        <v>1</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <f aca="false">AND(E20&gt;B20,F20&lt;C20)</f>
-        <v>1</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <f aca="false">AND(B20&gt;E20,C20&lt;F20)</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="0" t="n">
-        <f aca="false">OR(J20,K20)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="n">
         <v>0.819441132793889</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="7" t="n">
         <v>0.82015905363653</v>
       </c>
       <c r="D21" s="0" t="n">
@@ -1353,30 +984,10 @@
         <f aca="false">F21-E21</f>
         <v>0.000211036119999952</v>
       </c>
-      <c r="H21" s="0" t="n">
-        <f aca="false">F21&gt;=B21</f>
-        <v>1</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <f aca="false">E21&lt;=C21</f>
-        <v>1</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <f aca="false">AND(E21&gt;B21,F21&lt;C21)</f>
-        <v>1</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <f aca="false">AND(B21&gt;E21,C21&lt;F21)</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <f aca="false">OR(J21,K21)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.0130984209380457</v>
@@ -1398,30 +1009,10 @@
         <f aca="false">F22-E22</f>
         <v>5.86992899999882E-006</v>
       </c>
-      <c r="H22" s="0" t="n">
-        <f aca="false">F22&gt;=B22</f>
-        <v>1</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <f aca="false">E22&lt;=C22</f>
-        <v>1</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <f aca="false">AND(E22&gt;B22,F22&lt;C22)</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="0" t="n">
-        <f aca="false">AND(B22&gt;E22,C22&lt;F22)</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="0" t="n">
-        <f aca="false">OR(J22,K22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.991783353102071</v>
@@ -1443,25 +1034,103 @@
         <f aca="false">F23-E23</f>
         <v>4.70801700003243E-006</v>
       </c>
-      <c r="H23" s="0" t="n">
-        <f aca="false">F23&gt;=B23</f>
-        <v>1</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <f aca="false">E23&lt;=C23</f>
-        <v>1</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <f aca="false">AND(E23&gt;B23,F23&lt;C23)</f>
-        <v>1</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <f aca="false">AND(B23&gt;E23,C23&lt;F23)</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="0" t="n">
-        <f aca="false">OR(J23,K23)</f>
-        <v>1</v>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.016570078546</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0.017412420478</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">F25-E25</f>
+        <v>0.000842341931999998</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.016602244273</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.017474127532</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">F26-E26</f>
+        <v>0.000871883258999999</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.825699802309</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.826680913077</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">F27-E27</f>
+        <v>0.000981110768000004</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.98930638381</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0.990153253252</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">F28-E28</f>
+        <v>0.000846869441999965</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0.989292507364</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0.990183724592</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">F29-E29</f>
+        <v>0.000891217228000007</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1484,10 +1153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1497,17 +1166,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="10"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>30</v>
@@ -1521,225 +1190,225 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" s="10" t="n">
         <v>47.7934589385986</v>
       </c>
-      <c r="C3" s="11" t="n">
-        <v>28.5652449131012</v>
-      </c>
-      <c r="D3" s="11" t="n">
+      <c r="C3" s="0" t="n">
+        <v>28.6746640205383</v>
+      </c>
+      <c r="D3" s="10" t="n">
         <f aca="false">(B3-C3)/B3*100</f>
-        <v>40.2318945992178</v>
+        <v>40.002953003721</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10" t="n">
         <v>3337.95947337151</v>
       </c>
       <c r="C4" s="11" t="n">
-        <v>2846.65041542053</v>
-      </c>
-      <c r="D4" s="11" t="n">
+        <v>4669.08115720749</v>
+      </c>
+      <c r="D4" s="10" t="n">
         <f aca="false">(B4-C4)/B4*100</f>
-        <v>14.7188443080385</v>
+        <v>-39.878305727046</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="n">
         <v>3280.52771353722</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>2863.92050743103</v>
-      </c>
-      <c r="D5" s="11" t="n">
+        <v>4754.01056361198</v>
+      </c>
+      <c r="D5" s="10" t="n">
         <f aca="false">(B5-C5)/B5*100</f>
-        <v>12.6993960266527</v>
+        <v>-44.9160311615228</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10" t="n">
         <v>283.526683092117</v>
       </c>
-      <c r="C6" s="11" t="n">
-        <v>236.485964775085</v>
-      </c>
-      <c r="D6" s="11" t="n">
+      <c r="C6" s="0" t="n">
+        <v>236.775050401688</v>
+      </c>
+      <c r="D6" s="10" t="n">
         <f aca="false">(B6-C6)/B6*100</f>
-        <v>16.5912843912996</v>
+        <v>16.4893237492008</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10" t="n">
         <v>100.778197050095</v>
       </c>
-      <c r="C7" s="11" t="n">
-        <v>73.8054492473602</v>
-      </c>
-      <c r="D7" s="11" t="n">
+      <c r="C7" s="0" t="n">
+        <v>73.6161921024323</v>
+      </c>
+      <c r="D7" s="10" t="n">
         <f aca="false">(B7-C7)/B7*100</f>
-        <v>26.7644675061282</v>
+        <v>26.9522632302707</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10" t="n">
         <v>216.096117734909</v>
       </c>
-      <c r="C8" s="11" t="n">
-        <v>204.5092689991</v>
-      </c>
-      <c r="D8" s="11" t="n">
+      <c r="C8" s="0" t="n">
+        <v>210.310025215149</v>
+      </c>
+      <c r="D8" s="10" t="n">
         <f aca="false">(B8-C8)/B8*100</f>
-        <v>5.36189583471519</v>
+        <v>2.67755505300567</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B9" s="10" t="n">
         <v>2393.88133835793</v>
       </c>
-      <c r="C9" s="11" t="n">
-        <v>2142.34989571571</v>
-      </c>
-      <c r="D9" s="11" t="n">
+      <c r="C9" s="0" t="n">
+        <v>2109.79339981079</v>
+      </c>
+      <c r="D9" s="10" t="n">
         <f aca="false">(B9-C9)/B9*100</f>
-        <v>10.5072644417183</v>
+        <v>11.8672523151045</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B10" s="10" t="n">
         <v>2612.57214426994</v>
       </c>
-      <c r="C10" s="11" t="n">
-        <v>1866.81068682671</v>
-      </c>
-      <c r="D10" s="11" t="n">
+      <c r="C10" s="0" t="n">
+        <v>2262.65604710579</v>
+      </c>
+      <c r="D10" s="10" t="n">
         <f aca="false">(B10-C10)/B10*100</f>
-        <v>28.5451048339043</v>
+        <v>13.3935477315569</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10" t="n">
         <v>2417.28077697754</v>
       </c>
-      <c r="C11" s="11" t="n">
-        <v>2089.90823674202</v>
-      </c>
-      <c r="D11" s="11" t="n">
+      <c r="C11" s="0" t="n">
+        <v>2557.20226812363</v>
+      </c>
+      <c r="D11" s="10" t="n">
         <f aca="false">(B11-C11)/B11*100</f>
-        <v>13.543008464447</v>
+        <v>-5.7883838931214</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10" t="n">
         <v>192.995433092117</v>
       </c>
-      <c r="C12" s="11" t="n">
-        <v>138.85014629364</v>
-      </c>
-      <c r="D12" s="11" t="n">
+      <c r="C12" s="0" t="n">
+        <v>136.802144765854</v>
+      </c>
+      <c r="D12" s="10" t="n">
         <f aca="false">(B12-C12)/B12*100</f>
-        <v>28.055216608485</v>
+        <v>29.1163824065423</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" s="10" t="n">
         <v>230.411333799362</v>
       </c>
-      <c r="C13" s="11" t="n">
-        <v>154.65989613533</v>
-      </c>
-      <c r="D13" s="11" t="n">
+      <c r="C13" s="0" t="n">
+        <v>156.232561588287</v>
+      </c>
+      <c r="D13" s="10" t="n">
         <f aca="false">(B13-C13)/B13*100</f>
-        <v>32.8766108918908</v>
+        <v>32.1940639758929</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="B14" s="10" t="n">
         <v>2896.83513903618</v>
       </c>
-      <c r="C14" s="11" t="n">
-        <v>2441.3656680584</v>
-      </c>
-      <c r="D14" s="11" t="n">
+      <c r="C14" s="0" t="n">
+        <v>2452.60836696625</v>
+      </c>
+      <c r="D14" s="10" t="n">
         <f aca="false">(B14-C14)/B14*100</f>
-        <v>15.7230028329926</v>
+        <v>15.3349000115254</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10" t="n">
         <v>15.5867919921875</v>
       </c>
-      <c r="C15" s="11" t="n">
-        <v>3.41501140594482</v>
-      </c>
-      <c r="D15" s="11" t="n">
+      <c r="C15" s="0" t="n">
+        <v>3.44472551345825</v>
+      </c>
+      <c r="D15" s="10" t="n">
         <f aca="false">(B15-C15)/B15*100</f>
-        <v>78.0903510635382</v>
+        <v>77.8997146097488</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="B16" s="10" t="n">
         <v>52.7952065467835</v>
       </c>
-      <c r="C16" s="11" t="n">
-        <v>6.85991859436035</v>
-      </c>
-      <c r="D16" s="11" t="n">
+      <c r="C16" s="0" t="n">
+        <v>6.80246520042419</v>
+      </c>
+      <c r="D16" s="10" t="n">
         <f aca="false">(B16-C16)/B16*100</f>
-        <v>87.006550323311</v>
+        <v>87.1153734489204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1747,13 +1416,13 @@
       <c r="A18" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1761,76 +1430,141 @@
       <c r="A19" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="B20" s="10" t="n">
         <v>33.3790278434753</v>
       </c>
-      <c r="C20" s="11" t="n">
-        <v>62.635</v>
-      </c>
-      <c r="D20" s="11" t="n">
+      <c r="C20" s="0" t="n">
+        <v>59.8777592182159</v>
+      </c>
+      <c r="D20" s="10" t="n">
         <f aca="false">(B20-C20)/B20*100</f>
-        <v>-87.6477658178513</v>
+        <v>-79.3873671186633</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="B21" s="10" t="n">
         <v>419.473532438278</v>
       </c>
-      <c r="C21" s="11" t="n">
-        <v>588.402968406677</v>
-      </c>
-      <c r="D21" s="11" t="n">
+      <c r="C21" s="0" t="n">
+        <v>577.392343044281</v>
+      </c>
+      <c r="D21" s="10" t="n">
         <f aca="false">(B21-C21)/B21*100</f>
-        <v>-40.2717747139995</v>
+        <v>-37.6469069903091</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="B22" s="10" t="n">
         <v>1.53280353546143</v>
       </c>
-      <c r="C22" s="11" t="n">
-        <v>1.01343560218811</v>
-      </c>
-      <c r="D22" s="11" t="n">
+      <c r="C22" s="0" t="n">
+        <v>1.00603032112122</v>
+      </c>
+      <c r="D22" s="10" t="n">
         <f aca="false">(B22-C22)/B22*100</f>
-        <v>33.8835291841213</v>
+        <v>34.3666492249859</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>2.270343542099</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1.49850702285767</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <f aca="false">(B23-C23)/B23*100</f>
+        <v>33.9964637478497</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="11" t="n">
-        <v>2.270343542099</v>
-      </c>
-      <c r="C23" s="11" t="n">
-        <v>1.48863387107849</v>
-      </c>
-      <c r="D23" s="11" t="n">
-        <f aca="false">(B23-C23)/B23*100</f>
-        <v>34.4313385408534</v>
-      </c>
-    </row>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>4669.08115720749</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>4754.01056361198</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>2575.22144079208</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2489.62328386307</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>3231.90753269196</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1847,22 +1581,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1872,7 +1606,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
@@ -1886,7 +1620,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>85160</v>
@@ -1901,37 +1635,37 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3527020</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>2479199</v>
-      </c>
-      <c r="D4" s="12" t="n">
+        <v>2981764</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <f aca="false">C4-1</f>
-        <v>2479198</v>
+        <v>2981763</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3568525</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>2510758</v>
-      </c>
-      <c r="D5" s="12" t="n">
+        <v>3017679</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <f aca="false">C5-1</f>
-        <v>2510757</v>
+        <v>3017678</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>467635</v>
@@ -1939,14 +1673,14 @@
       <c r="C6" s="0" t="n">
         <v>490145</v>
       </c>
-      <c r="D6" s="12" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">C6-1</f>
         <v>490144</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>165043</v>
@@ -1954,14 +1688,14 @@
       <c r="C7" s="0" t="n">
         <v>175194</v>
       </c>
-      <c r="D7" s="12" t="n">
+      <c r="D7" s="0" t="n">
         <f aca="false">C7-1</f>
         <v>175193</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>406424</v>
@@ -1969,14 +1703,14 @@
       <c r="C8" s="0" t="n">
         <v>425443</v>
       </c>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="0" t="n">
         <f aca="false">C8-1</f>
         <v>425442</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2543695</v>
@@ -1984,39 +1718,39 @@
       <c r="C9" s="0" t="n">
         <v>1839612</v>
       </c>
-      <c r="D9" s="12" t="n">
+      <c r="D9" s="0" t="n">
         <f aca="false">C9-1</f>
         <v>1839611</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2813395</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>2083422</v>
-      </c>
-      <c r="D10" s="12" t="n">
+        <v>2234057</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <f aca="false">C10-1</f>
-        <v>2083421</v>
+        <v>2234056</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2829690</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>2177639</v>
-      </c>
-      <c r="D11" s="12" t="n">
+        <v>2331091</v>
+      </c>
+      <c r="D11" s="0" t="n">
         <f aca="false">C11-1</f>
-        <v>2177638</v>
+        <v>2331090</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>38</v>
@@ -2024,7 +1758,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>327687</v>
@@ -2032,7 +1766,7 @@
       <c r="C12" s="0" t="n">
         <v>337394</v>
       </c>
-      <c r="D12" s="12" t="n">
+      <c r="D12" s="0" t="n">
         <f aca="false">C12-1</f>
         <v>337393</v>
       </c>
@@ -2042,7 +1776,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>381372</v>
@@ -2050,7 +1784,7 @@
       <c r="C13" s="0" t="n">
         <v>381372</v>
       </c>
-      <c r="D13" s="12" t="n">
+      <c r="D13" s="0" t="n">
         <f aca="false">C13-1</f>
         <v>381371</v>
       </c>
@@ -2060,7 +1794,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>3006113</v>
@@ -2068,7 +1802,7 @@
       <c r="C14" s="0" t="n">
         <v>2302933</v>
       </c>
-      <c r="D14" s="12" t="n">
+      <c r="D14" s="0" t="n">
         <f aca="false">C14-1</f>
         <v>2302932</v>
       </c>
@@ -2078,7 +1812,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>21293</v>
@@ -2096,7 +1830,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>42469</v>
@@ -2168,7 +1902,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>187443</v>
@@ -2186,7 +1920,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1480045</v>
@@ -2204,7 +1938,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>4231</v>
@@ -2222,7 +1956,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6664</v>
@@ -2235,6 +1969,72 @@
         <v>6761</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2981764</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">C25-1</f>
+        <v>2981763</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>3017679</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">C26-1</f>
+        <v>3017678</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1969425</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">C27-1</f>
+        <v>1969424</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2312730</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">C28-1</f>
+        <v>2312729</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>2555018</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">C29-1</f>
+        <v>2555017</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:D1"/>

</xml_diff>